<commit_message>
update source using ui.ui
</commit_message>
<xml_diff>
--- a/ObjectDetection/ObjectDectecionWithOpenCV/testExcel/test.xlsx
+++ b/ObjectDetection/ObjectDectecionWithOpenCV/testExcel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -618,15 +619,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:I4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+  <dimension ref="C4:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>28</v>
       </c>
@@ -647,6 +648,53 @@
       </c>
       <c r="I4">
         <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>267</v>
+      </c>
+      <c r="D3">
+        <v>289</v>
+      </c>
+      <c r="E3">
+        <v>289</v>
+      </c>
+      <c r="J3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>37</v>
+      </c>
+      <c r="H9">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Latest Image Detect
</commit_message>
<xml_diff>
--- a/ObjectDetection/ObjectDectecionWithOpenCV/testExcel/test.xlsx
+++ b/ObjectDetection/ObjectDectecionWithOpenCV/testExcel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="8" activeTab="12"/>
+    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
     <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -667,15 +669,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+  <dimension ref="A3:K19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>267</v>
       </c>
@@ -689,7 +691,21 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <v>72</v>
+      </c>
+      <c r="G7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G9">
         <v>37</v>
       </c>
@@ -697,24 +713,194 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K10">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K13">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H14">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>54</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="E4">
+        <v>108</v>
+      </c>
+      <c r="G4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>67</v>
+      </c>
+      <c r="C22">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>